<commit_message>
Registro actualizado 2025-10-15 22:19:16.793979
</commit_message>
<xml_diff>
--- a/logs_negociacion.xlsx
+++ b/logs_negociacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,6 +504,16 @@
           <t>IP_Usuario</t>
         </is>
       </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>MensajeUsuario</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>RespuestaIA</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -562,6 +572,8 @@
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -620,13 +632,13 @@
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1000271912</t>
-        </is>
+      <c r="B4" t="n">
+        <v>1000271912</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -668,6 +680,66 @@
           <t>34.19.100.134</t>
         </is>
       </c>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-10-15 22:19:16</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1000274330</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Elian</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>TARJETA DE CRÉDITO</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>PRORROGA SIN PAGO</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>48 cuotas</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>34.19.100.134</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>The Dalles</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Oregon</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Registro actualización 2025-10-15 22:24:54
</commit_message>
<xml_diff>
--- a/logs_negociacion.xlsx
+++ b/logs_negociacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -689,10 +689,8 @@
           <t>2025-10-15 22:19:16</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1000274330</t>
-        </is>
+      <c r="B5" t="n">
+        <v>1000274330</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -741,6 +739,64 @@
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-10-15 22:24:54</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1000135120</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Leidy</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>TARJETA DE CRÉDITO</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>PRORROGA CON PAGO</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>48 cuotas</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>34.19.100.134</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>The Dalles</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Oregon</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Registro actualización 2025-10-15 22:31:31
</commit_message>
<xml_diff>
--- a/logs_negociacion.xlsx
+++ b/logs_negociacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -745,10 +745,8 @@
           <t>2025-10-15 22:24:54</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>1000135120</t>
-        </is>
+      <c r="B6" t="n">
+        <v>1000135120</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -797,6 +795,80 @@
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr"/>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-10-15 17:31:30</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1000127336</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Paula</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>TARJETA DE CRÉDITO</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>****4376</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>REDIFERIDO SIN PAGO</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>36 cuotas</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>34.19.100.134</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>The Dalles</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Oregon</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>2025-10-15 17:31:30</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>****4376</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>34.19.100.134</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Registro actualización 2025-10-15 22:31:47
</commit_message>
<xml_diff>
--- a/logs_negociacion.xlsx
+++ b/logs_negociacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -801,10 +801,8 @@
           <t>2025-10-15 17:31:30</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1000127336</t>
-        </is>
+      <c r="B7" t="n">
+        <v>1000127336</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -868,6 +866,80 @@
       </c>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-10-15 17:31:47</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1000127336</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Paula</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>TARJETA DE CRÉDITO</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>****4376</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>REDIFERIDO SIN PAGO</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>36 cuotas</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>34.19.100.134</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>The Dalles</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Oregon</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>2025-10-15 17:31:47</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>****4376</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>34.19.100.134</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Registro actualización 2025-10-15 22:34:31
</commit_message>
<xml_diff>
--- a/logs_negociacion.xlsx
+++ b/logs_negociacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -873,10 +873,8 @@
           <t>2025-10-15 17:31:47</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>1000127336</t>
-        </is>
+      <c r="B8" t="n">
+        <v>1000127336</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -940,6 +938,88 @@
       </c>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-10-15 17:34:31</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1000127336</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Paula</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>TARJETA DE CRÉDITO</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>****4376</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>REDIFERIDO SIN PAGO</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Chat IA</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>34.19.100.134</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>The Dalles</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Oregon</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>2025-10-15 17:34:31</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>****4376</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>34.19.100.134</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>no quiero nada</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Entiendo que a veces podemos sentirnos así. Si necesitas hablar de algo o si hay alguna inquietud que tengas, estoy aquí para escucharte y ayudarte en lo que necesites. ¿Hay algo más en lo que pueda asistirte?</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Registro actualización 2025-10-16 17:49:17
</commit_message>
<xml_diff>
--- a/logs_negociacion.xlsx
+++ b/logs_negociacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -945,10 +945,8 @@
           <t>2025-10-15 17:34:31</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>1000127336</t>
-        </is>
+      <c r="B9" t="n">
+        <v>1000127336</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -1020,6 +1018,80 @@
           <t>Entiendo que a veces podemos sentirnos así. Si necesitas hablar de algo o si hay alguna inquietud que tengas, estoy aquí para escucharte y ayudarte en lo que necesites. ¿Hay algo más en lo que pueda asistirte?</t>
         </is>
       </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-10-16 12:49:16</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1000274330</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Elian</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>TARJETA DE CRÉDITO</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>****0786</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>PRORROGA SIN PAGO</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>24 cuotas</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>35.197.92.111</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>The Dalles</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Oregon</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>2025-10-16 12:49:16</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>*****0786</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>35.197.92.111</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Registro actualización 2025-10-16 17:58:32
</commit_message>
<xml_diff>
--- a/logs_negociacion.xlsx
+++ b/logs_negociacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1025,10 +1025,8 @@
           <t>2025-10-16 12:49:16</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1000274330</t>
-        </is>
+      <c r="B10" t="n">
+        <v>1000274330</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1092,6 +1090,80 @@
       </c>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-10-16 12:58:32</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1000271912</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>TARJETA DE CRÉDITO</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>****6898</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>REESTRUCTURACION CON PAGO</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>60 cuotas</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>35.197.92.111</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>The Dalles</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Oregon</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>2025-10-16 12:58:32</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>****6898</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>35.197.92.111</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Registro actualización 2025-10-16 20:40:18
</commit_message>
<xml_diff>
--- a/logs_negociacion.xlsx
+++ b/logs_negociacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1097,10 +1097,8 @@
           <t>2025-10-16 12:58:32</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1000271912</t>
-        </is>
+      <c r="B11" t="n">
+        <v>1000271912</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1164,6 +1162,80 @@
       </c>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-10-16 15:40:17</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1000271912</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>TARJETA DE CRÉDITO</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>****6898</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>REESTRUCTURACION CON PAGO</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>24 cuotas</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>35.197.92.111</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>The Dalles</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Oregon</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>2025-10-16 15:40:17</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>****6898</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>35.197.92.111</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Registro actualización 2025-12-15 15:39:04
</commit_message>
<xml_diff>
--- a/logs_negociacion.xlsx
+++ b/logs_negociacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1169,10 +1169,8 @@
           <t>2025-10-16 15:40:17</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1000271912</t>
-        </is>
+      <c r="B12" t="n">
+        <v>1000271912</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1236,6 +1234,80 @@
       </c>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-12-15 10:39:04</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1000135120</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Leidy</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>TARJETA DE CRÉDITO</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>****9053</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>PRORROGA CON PAGO</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>12 cuotas</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>35.230.127.150</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>The Dalles</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Oregon</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>2025-12-15 10:39:04</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>*****9053</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>35.230.127.150</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Registro actualización 2025-12-16 15:50:27
</commit_message>
<xml_diff>
--- a/logs_negociacion.xlsx
+++ b/logs_negociacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1241,10 +1241,8 @@
           <t>2025-12-15 10:39:04</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1000135120</t>
-        </is>
+      <c r="B13" t="n">
+        <v>1000135120</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1308,6 +1306,80 @@
       </c>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-12-16 10:50:26</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1000135120</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Leidy</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>TARJETA DE CRÉDITO</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>****9053</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>PRORROGA CON PAGO</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>12 cuotas</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>35.197.92.111</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>The Dalles</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Oregon</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>2025-12-16 10:50:26</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>*****9053</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>35.197.92.111</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Registro actualización 2025-12-26 17:36:07
</commit_message>
<xml_diff>
--- a/logs_negociacion.xlsx
+++ b/logs_negociacion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1313,10 +1313,8 @@
           <t>2025-12-16 10:50:26</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>1000135120</t>
-        </is>
+      <c r="B14" t="n">
+        <v>1000135120</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1380,6 +1378,80 @@
       </c>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-12-26 12:36:06</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1000127336</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Paula</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>TARJETA DE CRÉDITO</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>****4376</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>REDIFERIDO SIN PAGO</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>12 cuotas</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>34.127.88.74</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>The Dalles</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Oregon</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>United States</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>2025-12-26 12:36:06</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>****4376</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>34.127.88.74</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>